<commit_message>
Fix assignment of 2mag reactors where biomass for calibrations was sourced from
</commit_message>
<xml_diff>
--- a/data/FullWellDescription.xlsx
+++ b/data/FullWellDescription.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\CIW Master\Masterarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osthege\Repos\carbtmodel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD54B104-6E45-4184-AC7D-6FDC0FF47F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -712,7 +711,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,23 +871,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -924,23 +906,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1116,16 +1081,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="D362" sqref="D362"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1119,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>220</v>
@@ -1175,7 +1140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>220</v>
@@ -1196,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>220</v>
       </c>
@@ -1216,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>220</v>
       </c>
@@ -1236,7 +1201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>220</v>
       </c>
@@ -1256,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>220</v>
       </c>
@@ -1276,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>220</v>
       </c>
@@ -1287,7 +1252,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>220</v>
       </c>
@@ -1298,7 +1263,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>220</v>
       </c>
@@ -1309,7 +1274,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>220</v>
       </c>
@@ -1317,7 +1282,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
         <v>178</v>
@@ -1326,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>220</v>
       </c>
@@ -1334,7 +1299,7 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
         <v>178</v>
@@ -1343,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>220</v>
       </c>
@@ -1351,7 +1316,7 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
         <v>178</v>
@@ -1360,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>220</v>
       </c>
@@ -1380,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>220</v>
       </c>
@@ -1400,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>220</v>
       </c>
@@ -1420,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>220</v>
       </c>
@@ -1440,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>220</v>
       </c>
@@ -1460,7 +1425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>220</v>
       </c>
@@ -1480,7 +1445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>220</v>
       </c>
@@ -1491,7 +1456,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>220</v>
       </c>
@@ -1502,7 +1467,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>220</v>
       </c>
@@ -1513,7 +1478,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>220</v>
       </c>
@@ -1521,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E23" t="s">
         <v>179</v>
@@ -1530,7 +1495,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>220</v>
       </c>
@@ -1538,7 +1503,7 @@
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="E24" t="s">
         <v>179</v>
@@ -1547,7 +1512,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>220</v>
       </c>
@@ -1555,7 +1520,7 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E25" t="s">
         <v>179</v>
@@ -1564,7 +1529,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>220</v>
       </c>
@@ -1584,7 +1549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>220</v>
       </c>
@@ -1604,7 +1569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>220</v>
       </c>
@@ -1624,7 +1589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>220</v>
       </c>
@@ -1644,7 +1609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>220</v>
       </c>
@@ -1664,7 +1629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>220</v>
       </c>
@@ -1684,7 +1649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>220</v>
       </c>
@@ -1695,7 +1660,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>220</v>
       </c>
@@ -1706,7 +1671,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>220</v>
       </c>
@@ -1717,7 +1682,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>220</v>
       </c>
@@ -1725,7 +1690,7 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
         <v>180</v>
@@ -1734,7 +1699,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>220</v>
       </c>
@@ -1742,7 +1707,7 @@
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E36" t="s">
         <v>180</v>
@@ -1751,7 +1716,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>220</v>
       </c>
@@ -1759,7 +1724,7 @@
         <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
         <v>180</v>
@@ -1768,7 +1733,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>220</v>
       </c>
@@ -1788,7 +1753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>220</v>
       </c>
@@ -1808,7 +1773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>220</v>
       </c>
@@ -1828,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>220</v>
       </c>
@@ -1848,7 +1813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>220</v>
       </c>
@@ -1868,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>220</v>
       </c>
@@ -1888,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>220</v>
       </c>
@@ -1899,7 +1864,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>220</v>
       </c>
@@ -1910,7 +1875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>220</v>
       </c>
@@ -1921,7 +1886,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>220</v>
       </c>
@@ -1929,7 +1894,7 @@
         <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
         <v>181</v>
@@ -1938,7 +1903,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>220</v>
       </c>
@@ -1946,7 +1911,7 @@
         <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="E48" t="s">
         <v>181</v>
@@ -1955,7 +1920,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>220</v>
       </c>
@@ -1963,7 +1928,7 @@
         <v>57</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E49" t="s">
         <v>181</v>
@@ -1972,7 +1937,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>220</v>
       </c>
@@ -1992,7 +1957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>220</v>
       </c>
@@ -2012,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>220</v>
       </c>
@@ -2032,7 +1997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>220</v>
       </c>
@@ -2052,7 +2017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>220</v>
       </c>
@@ -2072,7 +2037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>220</v>
       </c>
@@ -2092,7 +2057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>220</v>
       </c>
@@ -2103,7 +2068,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>220</v>
       </c>
@@ -2114,7 +2079,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>220</v>
       </c>
@@ -2125,7 +2090,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>220</v>
       </c>
@@ -2133,7 +2098,7 @@
         <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E59" t="s">
         <v>182</v>
@@ -2142,7 +2107,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>220</v>
       </c>
@@ -2150,7 +2115,7 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="E60" t="s">
         <v>182</v>
@@ -2159,7 +2124,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>220</v>
       </c>
@@ -2167,7 +2132,7 @@
         <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E61" t="s">
         <v>182</v>
@@ -2176,7 +2141,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>220</v>
       </c>
@@ -2196,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>220</v>
       </c>
@@ -2216,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>220</v>
       </c>
@@ -2236,7 +2201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>220</v>
       </c>
@@ -2256,7 +2221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>220</v>
       </c>
@@ -2276,7 +2241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>220</v>
       </c>
@@ -2296,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>220</v>
       </c>
@@ -2307,7 +2272,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>220</v>
       </c>
@@ -2318,7 +2283,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>220</v>
       </c>
@@ -2329,7 +2294,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>220</v>
       </c>
@@ -2337,7 +2302,7 @@
         <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E71" t="s">
         <v>183</v>
@@ -2346,7 +2311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>220</v>
       </c>
@@ -2354,7 +2319,7 @@
         <v>80</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E72" t="s">
         <v>183</v>
@@ -2363,7 +2328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>220</v>
       </c>
@@ -2371,7 +2336,7 @@
         <v>81</v>
       </c>
       <c r="D73" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E73" t="s">
         <v>183</v>
@@ -2380,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>220</v>
       </c>
@@ -2400,7 +2365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>220</v>
       </c>
@@ -2420,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>220</v>
       </c>
@@ -2440,7 +2405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>220</v>
       </c>
@@ -2460,7 +2425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>220</v>
       </c>
@@ -2480,7 +2445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>220</v>
       </c>
@@ -2500,7 +2465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>220</v>
       </c>
@@ -2511,7 +2476,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>220</v>
       </c>
@@ -2522,7 +2487,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>220</v>
       </c>
@@ -2533,7 +2498,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>220</v>
       </c>
@@ -2544,7 +2509,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>220</v>
       </c>
@@ -2555,7 +2520,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>220</v>
       </c>
@@ -2566,7 +2531,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>220</v>
       </c>
@@ -2586,7 +2551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>220</v>
       </c>
@@ -2606,7 +2571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>220</v>
       </c>
@@ -2626,7 +2591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>220</v>
       </c>
@@ -2646,7 +2611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>220</v>
       </c>
@@ -2666,7 +2631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>220</v>
       </c>
@@ -2686,7 +2651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>220</v>
       </c>
@@ -2697,7 +2662,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>220</v>
       </c>
@@ -2708,7 +2673,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>220</v>
       </c>
@@ -2719,7 +2684,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>220</v>
       </c>
@@ -2730,7 +2695,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>220</v>
       </c>
@@ -2741,7 +2706,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>220</v>
       </c>
@@ -2752,7 +2717,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>7</v>
       </c>
@@ -2772,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>7</v>
       </c>
@@ -2792,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>7</v>
       </c>
@@ -2812,7 +2777,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>7</v>
       </c>
@@ -2832,7 +2797,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>7</v>
       </c>
@@ -2852,7 +2817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>7</v>
       </c>
@@ -2872,7 +2837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>7</v>
       </c>
@@ -2883,7 +2848,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>7</v>
       </c>
@@ -2894,7 +2859,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>7</v>
       </c>
@@ -2905,7 +2870,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2878,7 @@
         <v>19</v>
       </c>
       <c r="D107" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="E107" t="s">
         <v>178</v>
@@ -2922,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>7</v>
       </c>
@@ -2930,7 +2895,7 @@
         <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="E108" t="s">
         <v>178</v>
@@ -2939,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>7</v>
       </c>
@@ -2947,7 +2912,7 @@
         <v>21</v>
       </c>
       <c r="D109" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E109" t="s">
         <v>178</v>
@@ -2956,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>7</v>
       </c>
@@ -2976,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>7</v>
       </c>
@@ -2996,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>7</v>
       </c>
@@ -3016,7 +2981,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>7</v>
       </c>
@@ -3036,7 +3001,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>7</v>
       </c>
@@ -3056,7 +3021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>7</v>
       </c>
@@ -3076,7 +3041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>7</v>
       </c>
@@ -3087,7 +3052,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>7</v>
       </c>
@@ -3098,7 +3063,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>7</v>
       </c>
@@ -3109,7 +3074,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>7</v>
       </c>
@@ -3117,7 +3082,7 @@
         <v>31</v>
       </c>
       <c r="D119" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E119" t="s">
         <v>179</v>
@@ -3126,7 +3091,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>7</v>
       </c>
@@ -3134,7 +3099,7 @@
         <v>32</v>
       </c>
       <c r="D120" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="E120" t="s">
         <v>179</v>
@@ -3143,7 +3108,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>7</v>
       </c>
@@ -3151,7 +3116,7 @@
         <v>33</v>
       </c>
       <c r="D121" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E121" t="s">
         <v>179</v>
@@ -3160,7 +3125,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>7</v>
       </c>
@@ -3180,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>7</v>
       </c>
@@ -3200,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>7</v>
       </c>
@@ -3220,7 +3185,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>7</v>
       </c>
@@ -3240,7 +3205,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>7</v>
       </c>
@@ -3260,7 +3225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>7</v>
       </c>
@@ -3280,7 +3245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>7</v>
       </c>
@@ -3291,7 +3256,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>7</v>
       </c>
@@ -3302,7 +3267,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>7</v>
       </c>
@@ -3313,7 +3278,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>7</v>
       </c>
@@ -3321,7 +3286,7 @@
         <v>43</v>
       </c>
       <c r="D131" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="E131" t="s">
         <v>180</v>
@@ -3330,7 +3295,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>7</v>
       </c>
@@ -3338,7 +3303,7 @@
         <v>44</v>
       </c>
       <c r="D132" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E132" t="s">
         <v>180</v>
@@ -3347,7 +3312,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>7</v>
       </c>
@@ -3355,7 +3320,7 @@
         <v>45</v>
       </c>
       <c r="D133" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E133" t="s">
         <v>180</v>
@@ -3364,7 +3329,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>7</v>
       </c>
@@ -3384,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>7</v>
       </c>
@@ -3404,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>7</v>
       </c>
@@ -3424,7 +3389,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>7</v>
       </c>
@@ -3444,7 +3409,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>7</v>
       </c>
@@ -3464,7 +3429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>7</v>
       </c>
@@ -3484,7 +3449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>7</v>
       </c>
@@ -3495,7 +3460,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>7</v>
       </c>
@@ -3506,7 +3471,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>7</v>
       </c>
@@ -3517,7 +3482,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>7</v>
       </c>
@@ -3525,7 +3490,7 @@
         <v>55</v>
       </c>
       <c r="D143" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E143" t="s">
         <v>181</v>
@@ -3534,7 +3499,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>7</v>
       </c>
@@ -3542,7 +3507,7 @@
         <v>56</v>
       </c>
       <c r="D144" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="E144" t="s">
         <v>181</v>
@@ -3551,7 +3516,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>7</v>
       </c>
@@ -3559,7 +3524,7 @@
         <v>57</v>
       </c>
       <c r="D145" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E145" t="s">
         <v>181</v>
@@ -3568,7 +3533,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>7</v>
       </c>
@@ -3588,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>7</v>
       </c>
@@ -3608,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>7</v>
       </c>
@@ -3628,7 +3593,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>7</v>
       </c>
@@ -3648,7 +3613,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>7</v>
       </c>
@@ -3668,7 +3633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>7</v>
       </c>
@@ -3688,7 +3653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>7</v>
       </c>
@@ -3699,7 +3664,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>7</v>
       </c>
@@ -3710,7 +3675,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>7</v>
       </c>
@@ -3721,7 +3686,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>7</v>
       </c>
@@ -3729,7 +3694,7 @@
         <v>67</v>
       </c>
       <c r="D155" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E155" t="s">
         <v>182</v>
@@ -3738,7 +3703,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>7</v>
       </c>
@@ -3746,7 +3711,7 @@
         <v>68</v>
       </c>
       <c r="D156" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="E156" t="s">
         <v>182</v>
@@ -3755,7 +3720,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>7</v>
       </c>
@@ -3763,7 +3728,7 @@
         <v>69</v>
       </c>
       <c r="D157" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E157" t="s">
         <v>182</v>
@@ -3772,7 +3737,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>7</v>
       </c>
@@ -3792,7 +3757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>7</v>
       </c>
@@ -3812,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>7</v>
       </c>
@@ -3832,7 +3797,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>7</v>
       </c>
@@ -3852,7 +3817,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>7</v>
       </c>
@@ -3872,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>7</v>
       </c>
@@ -3892,7 +3857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>7</v>
       </c>
@@ -3903,7 +3868,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +3879,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>7</v>
       </c>
@@ -3925,7 +3890,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>7</v>
       </c>
@@ -3933,7 +3898,7 @@
         <v>79</v>
       </c>
       <c r="D167" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E167" t="s">
         <v>183</v>
@@ -3942,7 +3907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>7</v>
       </c>
@@ -3950,7 +3915,7 @@
         <v>80</v>
       </c>
       <c r="D168" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E168" t="s">
         <v>183</v>
@@ -3959,7 +3924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>7</v>
       </c>
@@ -3967,7 +3932,7 @@
         <v>81</v>
       </c>
       <c r="D169" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E169" t="s">
         <v>183</v>
@@ -3976,7 +3941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>7</v>
       </c>
@@ -3996,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>7</v>
       </c>
@@ -4016,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>7</v>
       </c>
@@ -4036,7 +4001,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>7</v>
       </c>
@@ -4056,7 +4021,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>7</v>
       </c>
@@ -4076,7 +4041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>7</v>
       </c>
@@ -4096,7 +4061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>7</v>
       </c>
@@ -4107,7 +4072,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4083,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>7</v>
       </c>
@@ -4129,7 +4094,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>7</v>
       </c>
@@ -4140,7 +4105,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>7</v>
       </c>
@@ -4151,7 +4116,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>7</v>
       </c>
@@ -4162,7 +4127,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>7</v>
       </c>
@@ -4182,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>7</v>
       </c>
@@ -4202,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>7</v>
       </c>
@@ -4222,7 +4187,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>7</v>
       </c>
@@ -4242,7 +4207,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>7</v>
       </c>
@@ -4262,7 +4227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>7</v>
       </c>
@@ -4282,7 +4247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>7</v>
       </c>
@@ -4293,7 +4258,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>7</v>
       </c>
@@ -4304,7 +4269,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>7</v>
       </c>
@@ -4315,7 +4280,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>7</v>
       </c>
@@ -4326,7 +4291,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>7</v>
       </c>
@@ -4337,7 +4302,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>7</v>
       </c>
@@ -4348,7 +4313,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>8</v>
       </c>
@@ -4368,7 +4333,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>8</v>
       </c>
@@ -4388,7 +4353,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>8</v>
       </c>
@@ -4408,7 +4373,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>8</v>
       </c>
@@ -4428,7 +4393,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>8</v>
       </c>
@@ -4448,7 +4413,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>8</v>
       </c>
@@ -4468,7 +4433,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>8</v>
       </c>
@@ -4479,7 +4444,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>8</v>
       </c>
@@ -4490,7 +4455,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>8</v>
       </c>
@@ -4501,7 +4466,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>8</v>
       </c>
@@ -4509,7 +4474,7 @@
         <v>19</v>
       </c>
       <c r="D203" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="E203" t="s">
         <v>178</v>
@@ -4518,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>8</v>
       </c>
@@ -4526,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="D204" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="E204" t="s">
         <v>178</v>
@@ -4535,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>8</v>
       </c>
@@ -4543,7 +4508,7 @@
         <v>21</v>
       </c>
       <c r="D205" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E205" t="s">
         <v>178</v>
@@ -4552,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>8</v>
       </c>
@@ -4572,7 +4537,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>8</v>
       </c>
@@ -4592,7 +4557,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>8</v>
       </c>
@@ -4612,7 +4577,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>8</v>
       </c>
@@ -4632,7 +4597,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>8</v>
       </c>
@@ -4652,7 +4617,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>8</v>
       </c>
@@ -4672,7 +4637,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>8</v>
       </c>
@@ -4683,7 +4648,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B213" t="s">
         <v>8</v>
       </c>
@@ -4694,7 +4659,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B214" t="s">
         <v>8</v>
       </c>
@@ -4705,7 +4670,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B215" t="s">
         <v>8</v>
       </c>
@@ -4713,7 +4678,7 @@
         <v>31</v>
       </c>
       <c r="D215" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E215" t="s">
         <v>179</v>
@@ -4722,7 +4687,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B216" t="s">
         <v>8</v>
       </c>
@@ -4730,7 +4695,7 @@
         <v>32</v>
       </c>
       <c r="D216" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="E216" t="s">
         <v>179</v>
@@ -4739,7 +4704,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B217" t="s">
         <v>8</v>
       </c>
@@ -4747,7 +4712,7 @@
         <v>33</v>
       </c>
       <c r="D217" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E217" t="s">
         <v>179</v>
@@ -4756,7 +4721,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B218" t="s">
         <v>8</v>
       </c>
@@ -4776,7 +4741,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B219" t="s">
         <v>8</v>
       </c>
@@ -4796,7 +4761,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B220" t="s">
         <v>8</v>
       </c>
@@ -4816,7 +4781,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B221" t="s">
         <v>8</v>
       </c>
@@ -4836,7 +4801,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B222" t="s">
         <v>8</v>
       </c>
@@ -4856,7 +4821,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B223" t="s">
         <v>8</v>
       </c>
@@ -4876,7 +4841,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B224" t="s">
         <v>8</v>
       </c>
@@ -4887,7 +4852,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B225" t="s">
         <v>8</v>
       </c>
@@ -4898,7 +4863,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B226" t="s">
         <v>8</v>
       </c>
@@ -4909,7 +4874,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B227" t="s">
         <v>8</v>
       </c>
@@ -4917,7 +4882,7 @@
         <v>43</v>
       </c>
       <c r="D227" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="E227" t="s">
         <v>180</v>
@@ -4926,7 +4891,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B228" t="s">
         <v>8</v>
       </c>
@@ -4934,7 +4899,7 @@
         <v>44</v>
       </c>
       <c r="D228" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E228" t="s">
         <v>180</v>
@@ -4943,7 +4908,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B229" t="s">
         <v>8</v>
       </c>
@@ -4951,7 +4916,7 @@
         <v>45</v>
       </c>
       <c r="D229" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E229" t="s">
         <v>180</v>
@@ -4960,7 +4925,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B230" t="s">
         <v>8</v>
       </c>
@@ -4980,7 +4945,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B231" t="s">
         <v>8</v>
       </c>
@@ -5000,7 +4965,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="232" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B232" t="s">
         <v>8</v>
       </c>
@@ -5020,7 +4985,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B233" t="s">
         <v>8</v>
       </c>
@@ -5040,7 +5005,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B234" t="s">
         <v>8</v>
       </c>
@@ -5060,7 +5025,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="235" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B235" t="s">
         <v>8</v>
       </c>
@@ -5080,7 +5045,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="236" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B236" t="s">
         <v>8</v>
       </c>
@@ -5091,7 +5056,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B237" t="s">
         <v>8</v>
       </c>
@@ -5102,7 +5067,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="238" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B238" t="s">
         <v>8</v>
       </c>
@@ -5113,7 +5078,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B239" t="s">
         <v>8</v>
       </c>
@@ -5121,7 +5086,7 @@
         <v>55</v>
       </c>
       <c r="D239" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E239" t="s">
         <v>181</v>
@@ -5130,7 +5095,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B240" t="s">
         <v>8</v>
       </c>
@@ -5138,7 +5103,7 @@
         <v>56</v>
       </c>
       <c r="D240" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="E240" t="s">
         <v>181</v>
@@ -5147,7 +5112,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B241" t="s">
         <v>8</v>
       </c>
@@ -5155,7 +5120,7 @@
         <v>57</v>
       </c>
       <c r="D241" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E241" t="s">
         <v>181</v>
@@ -5164,7 +5129,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B242" t="s">
         <v>8</v>
       </c>
@@ -5184,7 +5149,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B243" t="s">
         <v>8</v>
       </c>
@@ -5204,7 +5169,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B244" t="s">
         <v>8</v>
       </c>
@@ -5224,7 +5189,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B245" t="s">
         <v>8</v>
       </c>
@@ -5244,7 +5209,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B246" t="s">
         <v>8</v>
       </c>
@@ -5264,7 +5229,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B247" t="s">
         <v>8</v>
       </c>
@@ -5284,7 +5249,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B248" t="s">
         <v>8</v>
       </c>
@@ -5295,7 +5260,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B249" t="s">
         <v>8</v>
       </c>
@@ -5306,7 +5271,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B250" t="s">
         <v>8</v>
       </c>
@@ -5317,7 +5282,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B251" t="s">
         <v>8</v>
       </c>
@@ -5325,7 +5290,7 @@
         <v>67</v>
       </c>
       <c r="D251" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E251" t="s">
         <v>182</v>
@@ -5334,7 +5299,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B252" t="s">
         <v>8</v>
       </c>
@@ -5342,7 +5307,7 @@
         <v>68</v>
       </c>
       <c r="D252" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="E252" t="s">
         <v>182</v>
@@ -5351,7 +5316,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B253" t="s">
         <v>8</v>
       </c>
@@ -5359,7 +5324,7 @@
         <v>69</v>
       </c>
       <c r="D253" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E253" t="s">
         <v>182</v>
@@ -5368,7 +5333,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B254" t="s">
         <v>8</v>
       </c>
@@ -5388,7 +5353,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B255" t="s">
         <v>8</v>
       </c>
@@ -5408,7 +5373,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B256" t="s">
         <v>8</v>
       </c>
@@ -5428,7 +5393,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B257" t="s">
         <v>8</v>
       </c>
@@ -5448,7 +5413,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B258" t="s">
         <v>8</v>
       </c>
@@ -5468,7 +5433,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B259" t="s">
         <v>8</v>
       </c>
@@ -5488,7 +5453,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
         <v>8</v>
       </c>
@@ -5499,7 +5464,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B261" t="s">
         <v>8</v>
       </c>
@@ -5510,7 +5475,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B262" t="s">
         <v>8</v>
       </c>
@@ -5521,7 +5486,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B263" t="s">
         <v>8</v>
       </c>
@@ -5529,7 +5494,7 @@
         <v>79</v>
       </c>
       <c r="D263" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E263" t="s">
         <v>183</v>
@@ -5538,7 +5503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B264" t="s">
         <v>8</v>
       </c>
@@ -5546,7 +5511,7 @@
         <v>80</v>
       </c>
       <c r="D264" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E264" t="s">
         <v>183</v>
@@ -5555,7 +5520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B265" t="s">
         <v>8</v>
       </c>
@@ -5563,7 +5528,7 @@
         <v>81</v>
       </c>
       <c r="D265" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E265" t="s">
         <v>183</v>
@@ -5572,7 +5537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B266" t="s">
         <v>8</v>
       </c>
@@ -5592,7 +5557,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="267" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B267" t="s">
         <v>8</v>
       </c>
@@ -5612,7 +5577,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="268" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B268" t="s">
         <v>8</v>
       </c>
@@ -5632,7 +5597,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="269" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B269" t="s">
         <v>8</v>
       </c>
@@ -5652,7 +5617,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="270" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B270" t="s">
         <v>8</v>
       </c>
@@ -5672,7 +5637,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="271" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B271" t="s">
         <v>8</v>
       </c>
@@ -5692,7 +5657,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B272" t="s">
         <v>8</v>
       </c>
@@ -5703,7 +5668,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="273" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B273" t="s">
         <v>8</v>
       </c>
@@ -5714,7 +5679,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="274" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B274" t="s">
         <v>8</v>
       </c>
@@ -5725,7 +5690,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B275" t="s">
         <v>8</v>
       </c>
@@ -5736,7 +5701,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="276" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B276" t="s">
         <v>8</v>
       </c>
@@ -5747,7 +5712,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="277" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B277" t="s">
         <v>8</v>
       </c>
@@ -5758,7 +5723,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="278" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B278" t="s">
         <v>8</v>
       </c>
@@ -5778,7 +5743,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="279" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B279" t="s">
         <v>8</v>
       </c>
@@ -5798,7 +5763,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="280" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B280" t="s">
         <v>8</v>
       </c>
@@ -5818,7 +5783,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="281" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B281" t="s">
         <v>8</v>
       </c>
@@ -5838,7 +5803,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="282" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B282" t="s">
         <v>8</v>
       </c>
@@ -5858,7 +5823,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="283" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B283" t="s">
         <v>8</v>
       </c>
@@ -5878,7 +5843,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="284" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B284" t="s">
         <v>8</v>
       </c>
@@ -5889,7 +5854,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B285" t="s">
         <v>8</v>
       </c>
@@ -5900,7 +5865,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="286" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B286" t="s">
         <v>8</v>
       </c>
@@ -5911,7 +5876,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B287" t="s">
         <v>8</v>
       </c>
@@ -5922,7 +5887,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="288" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B288" t="s">
         <v>8</v>
       </c>
@@ -5933,7 +5898,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="289" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B289" t="s">
         <v>8</v>
       </c>
@@ -5944,7 +5909,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="290" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B290" t="s">
         <v>9</v>
       </c>
@@ -5964,7 +5929,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B291" t="s">
         <v>9</v>
       </c>
@@ -5984,7 +5949,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="292" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B292" t="s">
         <v>9</v>
       </c>
@@ -6004,7 +5969,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="293" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B293" t="s">
         <v>9</v>
       </c>
@@ -6024,7 +5989,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="294" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B294" t="s">
         <v>9</v>
       </c>
@@ -6044,7 +6009,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="295" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B295" t="s">
         <v>9</v>
       </c>
@@ -6064,7 +6029,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="296" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B296" t="s">
         <v>9</v>
       </c>
@@ -6075,7 +6040,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="297" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B297" t="s">
         <v>9</v>
       </c>
@@ -6086,7 +6051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B298" t="s">
         <v>9</v>
       </c>
@@ -6097,7 +6062,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="299" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B299" t="s">
         <v>9</v>
       </c>
@@ -6105,7 +6070,7 @@
         <v>19</v>
       </c>
       <c r="D299" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="E299" t="s">
         <v>178</v>
@@ -6114,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B300" t="s">
         <v>9</v>
       </c>
@@ -6122,7 +6087,7 @@
         <v>20</v>
       </c>
       <c r="D300" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="E300" t="s">
         <v>178</v>
@@ -6131,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B301" t="s">
         <v>9</v>
       </c>
@@ -6139,7 +6104,7 @@
         <v>21</v>
       </c>
       <c r="D301" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E301" t="s">
         <v>178</v>
@@ -6148,7 +6113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B302" t="s">
         <v>9</v>
       </c>
@@ -6168,7 +6133,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="303" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B303" t="s">
         <v>9</v>
       </c>
@@ -6188,7 +6153,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="304" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B304" t="s">
         <v>9</v>
       </c>
@@ -6208,7 +6173,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="305" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B305" t="s">
         <v>9</v>
       </c>
@@ -6228,7 +6193,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="306" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B306" t="s">
         <v>9</v>
       </c>
@@ -6248,7 +6213,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="307" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B307" t="s">
         <v>9</v>
       </c>
@@ -6268,7 +6233,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="308" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B308" t="s">
         <v>9</v>
       </c>
@@ -6279,7 +6244,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="309" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B309" t="s">
         <v>9</v>
       </c>
@@ -6290,7 +6255,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="310" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B310" t="s">
         <v>9</v>
       </c>
@@ -6301,7 +6266,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="311" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B311" t="s">
         <v>9</v>
       </c>
@@ -6309,7 +6274,7 @@
         <v>31</v>
       </c>
       <c r="D311" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E311" t="s">
         <v>179</v>
@@ -6318,7 +6283,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="312" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B312" t="s">
         <v>9</v>
       </c>
@@ -6326,7 +6291,7 @@
         <v>32</v>
       </c>
       <c r="D312" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="E312" t="s">
         <v>179</v>
@@ -6335,7 +6300,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="313" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B313" t="s">
         <v>9</v>
       </c>
@@ -6343,7 +6308,7 @@
         <v>33</v>
       </c>
       <c r="D313" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E313" t="s">
         <v>179</v>
@@ -6352,7 +6317,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="314" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B314" t="s">
         <v>9</v>
       </c>
@@ -6372,7 +6337,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="315" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B315" t="s">
         <v>9</v>
       </c>
@@ -6392,7 +6357,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="316" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B316" t="s">
         <v>9</v>
       </c>
@@ -6412,7 +6377,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="317" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B317" t="s">
         <v>9</v>
       </c>
@@ -6432,7 +6397,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="318" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B318" t="s">
         <v>9</v>
       </c>
@@ -6452,7 +6417,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="319" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B319" t="s">
         <v>9</v>
       </c>
@@ -6472,7 +6437,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="320" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B320" t="s">
         <v>9</v>
       </c>
@@ -6483,7 +6448,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B321" t="s">
         <v>9</v>
       </c>
@@ -6494,7 +6459,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B322" t="s">
         <v>9</v>
       </c>
@@ -6505,7 +6470,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="323" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B323" t="s">
         <v>9</v>
       </c>
@@ -6513,7 +6478,7 @@
         <v>43</v>
       </c>
       <c r="D323" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="E323" t="s">
         <v>180</v>
@@ -6522,7 +6487,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B324" t="s">
         <v>9</v>
       </c>
@@ -6530,7 +6495,7 @@
         <v>44</v>
       </c>
       <c r="D324" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E324" t="s">
         <v>180</v>
@@ -6539,7 +6504,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B325" t="s">
         <v>9</v>
       </c>
@@ -6547,7 +6512,7 @@
         <v>45</v>
       </c>
       <c r="D325" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E325" t="s">
         <v>180</v>
@@ -6556,7 +6521,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B326" t="s">
         <v>9</v>
       </c>
@@ -6576,7 +6541,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B327" t="s">
         <v>9</v>
       </c>
@@ -6596,7 +6561,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B328" t="s">
         <v>9</v>
       </c>
@@ -6616,7 +6581,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="329" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B329" t="s">
         <v>9</v>
       </c>
@@ -6636,7 +6601,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="330" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B330" t="s">
         <v>9</v>
       </c>
@@ -6656,7 +6621,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="331" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B331" t="s">
         <v>9</v>
       </c>
@@ -6676,7 +6641,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B332" t="s">
         <v>9</v>
       </c>
@@ -6687,7 +6652,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B333" t="s">
         <v>9</v>
       </c>
@@ -6698,7 +6663,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="334" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B334" t="s">
         <v>9</v>
       </c>
@@ -6709,7 +6674,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="335" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B335" t="s">
         <v>9</v>
       </c>
@@ -6717,7 +6682,7 @@
         <v>55</v>
       </c>
       <c r="D335" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E335" t="s">
         <v>181</v>
@@ -6726,7 +6691,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="336" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B336" t="s">
         <v>9</v>
       </c>
@@ -6734,7 +6699,7 @@
         <v>56</v>
       </c>
       <c r="D336" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="E336" t="s">
         <v>181</v>
@@ -6743,7 +6708,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="337" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B337" t="s">
         <v>9</v>
       </c>
@@ -6751,7 +6716,7 @@
         <v>57</v>
       </c>
       <c r="D337" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E337" t="s">
         <v>181</v>
@@ -6760,7 +6725,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="338" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B338" t="s">
         <v>9</v>
       </c>
@@ -6780,7 +6745,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="339" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B339" t="s">
         <v>9</v>
       </c>
@@ -6800,7 +6765,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="340" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B340" t="s">
         <v>9</v>
       </c>
@@ -6820,7 +6785,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="341" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B341" t="s">
         <v>9</v>
       </c>
@@ -6840,7 +6805,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="342" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B342" t="s">
         <v>9</v>
       </c>
@@ -6860,7 +6825,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="343" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B343" t="s">
         <v>9</v>
       </c>
@@ -6880,7 +6845,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="344" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B344" t="s">
         <v>9</v>
       </c>
@@ -6891,7 +6856,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="345" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B345" t="s">
         <v>9</v>
       </c>
@@ -6902,7 +6867,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="346" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B346" t="s">
         <v>9</v>
       </c>
@@ -6913,7 +6878,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="347" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B347" t="s">
         <v>9</v>
       </c>
@@ -6921,7 +6886,7 @@
         <v>67</v>
       </c>
       <c r="D347" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E347" t="s">
         <v>182</v>
@@ -6930,7 +6895,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="348" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B348" t="s">
         <v>9</v>
       </c>
@@ -6938,7 +6903,7 @@
         <v>68</v>
       </c>
       <c r="D348" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="E348" t="s">
         <v>182</v>
@@ -6947,7 +6912,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="349" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B349" t="s">
         <v>9</v>
       </c>
@@ -6955,7 +6920,7 @@
         <v>69</v>
       </c>
       <c r="D349" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E349" t="s">
         <v>182</v>
@@ -6964,7 +6929,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="350" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B350" t="s">
         <v>9</v>
       </c>
@@ -6984,7 +6949,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="351" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B351" t="s">
         <v>9</v>
       </c>
@@ -7004,7 +6969,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="352" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B352" t="s">
         <v>9</v>
       </c>
@@ -7024,7 +6989,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="353" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B353" t="s">
         <v>9</v>
       </c>
@@ -7044,7 +7009,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="354" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B354" t="s">
         <v>9</v>
       </c>
@@ -7064,7 +7029,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="355" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B355" t="s">
         <v>9</v>
       </c>
@@ -7084,7 +7049,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="356" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B356" t="s">
         <v>9</v>
       </c>
@@ -7095,7 +7060,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="357" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B357" t="s">
         <v>9</v>
       </c>
@@ -7106,7 +7071,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="358" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B358" t="s">
         <v>9</v>
       </c>
@@ -7117,7 +7082,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="359" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B359" t="s">
         <v>9</v>
       </c>
@@ -7125,7 +7090,7 @@
         <v>79</v>
       </c>
       <c r="D359" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E359" t="s">
         <v>183</v>
@@ -7134,7 +7099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="360" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B360" t="s">
         <v>9</v>
       </c>
@@ -7142,7 +7107,7 @@
         <v>80</v>
       </c>
       <c r="D360" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E360" t="s">
         <v>183</v>
@@ -7151,7 +7116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B361" t="s">
         <v>9</v>
       </c>
@@ -7159,7 +7124,7 @@
         <v>81</v>
       </c>
       <c r="D361" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E361" t="s">
         <v>183</v>
@@ -7168,7 +7133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="362" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B362" t="s">
         <v>9</v>
       </c>
@@ -7188,7 +7153,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="363" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B363" t="s">
         <v>9</v>
       </c>
@@ -7208,7 +7173,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="364" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B364" t="s">
         <v>9</v>
       </c>
@@ -7228,7 +7193,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="365" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B365" t="s">
         <v>9</v>
       </c>
@@ -7248,7 +7213,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="366" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B366" t="s">
         <v>9</v>
       </c>
@@ -7268,7 +7233,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="367" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B367" t="s">
         <v>9</v>
       </c>
@@ -7288,7 +7253,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="368" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B368" t="s">
         <v>9</v>
       </c>
@@ -7299,7 +7264,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="369" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B369" t="s">
         <v>9</v>
       </c>
@@ -7310,7 +7275,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="370" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B370" t="s">
         <v>9</v>
       </c>
@@ -7321,7 +7286,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="371" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B371" t="s">
         <v>9</v>
       </c>
@@ -7332,7 +7297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="372" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B372" t="s">
         <v>9</v>
       </c>
@@ -7343,7 +7308,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="373" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B373" t="s">
         <v>9</v>
       </c>
@@ -7354,7 +7319,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="374" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B374" t="s">
         <v>9</v>
       </c>
@@ -7374,7 +7339,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="375" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B375" t="s">
         <v>9</v>
       </c>
@@ -7394,7 +7359,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="376" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B376" t="s">
         <v>9</v>
       </c>
@@ -7414,7 +7379,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="377" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B377" t="s">
         <v>9</v>
       </c>
@@ -7434,7 +7399,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="378" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B378" t="s">
         <v>9</v>
       </c>
@@ -7454,7 +7419,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="379" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B379" t="s">
         <v>9</v>
       </c>
@@ -7474,7 +7439,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="380" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B380" t="s">
         <v>9</v>
       </c>
@@ -7485,7 +7450,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="381" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B381" t="s">
         <v>9</v>
       </c>
@@ -7496,7 +7461,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="382" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B382" t="s">
         <v>9</v>
       </c>
@@ -7507,7 +7472,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="383" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B383" t="s">
         <v>9</v>
       </c>
@@ -7518,7 +7483,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="384" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B384" t="s">
         <v>9</v>
       </c>
@@ -7529,7 +7494,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B385" t="s">
         <v>9</v>
       </c>

</xml_diff>